<commit_message>
Control code & matlab
</commit_message>
<xml_diff>
--- a/Control/Typify/ParametrosMotores.xlsx
+++ b/Control/Typify/ParametrosMotores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yovan\Desktop\Universidad\2024-I\Servomecanismos\Servomechanisms_projects\Control\Typify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234B5729-F992-4006-B7AC-7591E46A6A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2FE9C2-42CC-491A-9484-528F6F760256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{EC05CA1B-F2B3-4E35-871B-95D20DD1E04C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EC05CA1B-F2B3-4E35-871B-95D20DD1E04C}"/>
   </bookViews>
   <sheets>
     <sheet name="M1" sheetId="1" r:id="rId1"/>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D753628-B62A-4FBA-A418-C4CB7F20AF98}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,13 +810,13 @@
       </c>
       <c r="B24" s="1">
         <f>(1/(2*SQRT($B$21*$D$21*D24)))*($B$21*E24+1)</f>
-        <v>0.79898453325073471</v>
+        <v>0.80152380005075563</v>
       </c>
       <c r="D24" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1">
-        <v>1.03</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF7D9CA-D51A-4738-937B-B3A18F293B88}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>

</xml_diff>